<commit_message>
updated test data and added one more test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Data.xlsx
+++ b/src/test/resources/TestData/Data.xlsx
@@ -3,33 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272A2262-1C39-47CE-9A3C-5EDAB9B8207D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88640029-B654-4743-89DA-D9CDB804D249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
-    <sheet name="TestData" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>ProductAddToCartTest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Product_Category</t>
   </si>
@@ -456,46 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +457,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -516,36 +467,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added the code to compare the confirmation message text
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Data.xlsx
+++ b/src/test/resources/TestData/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88640029-B654-4743-89DA-D9CDB804D249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F04843-AF80-414F-987F-0AD817908143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Product_Category</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t>verifyProductSelection</t>
+  </si>
+  <si>
+    <t>verifyProductAddedInCartConfirmationMessage</t>
+  </si>
+  <si>
+    <t>Confirmation_Message</t>
+  </si>
+  <si>
+    <t>Added to Cart</t>
   </si>
 </sst>
 </file>
@@ -443,15 +452,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,6 +488,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>